<commit_message>
Corregido typo y añadida estación de bicicletas por issue sociedad-bienestar-equipamientos-municipales#10
</commit_message>
<xml_diff>
--- a/urbanismo-infraestructuras/equipamiento/tipo-equipamiento.xlsx
+++ b/urbanismo-infraestructuras/equipamiento/tipo-equipamiento.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="260">
   <si>
     <t>Equipamiento Cultural</t>
   </si>
@@ -797,6 +797,12 @@
   </si>
   <si>
     <t>Equipamiento Educativo</t>
+  </si>
+  <si>
+    <t>Estación de esquí alpino</t>
+  </si>
+  <si>
+    <t>Estación de bicicletas</t>
   </si>
 </sst>
 </file>
@@ -960,13 +966,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1026,38 +1033,39 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="32">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="31" builtinId="9" hidden="1"/>
+  <cellStyles count="33">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1325,7 +1333,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1333,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D213"/>
+  <dimension ref="B1:D214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="C215" sqref="C215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2367,7 +2375,7 @@
       <c r="B145" s="8"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>95</v>
+        <v>258</v>
       </c>
     </row>
     <row r="146" spans="2:4">
@@ -2840,11 +2848,18 @@
         <v>244</v>
       </c>
     </row>
+    <row r="214" spans="2:3">
+      <c r="B214" s="6"/>
+      <c r="C214" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B39" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>